<commit_message>
Verification Faite sur plateforme
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE_08_Plateforme.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE_08_Plateforme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="tblPlateforme" sheetId="1" r:id="rId1"/>
@@ -56,15 +56,9 @@
     <t>Alienware15</t>
   </si>
   <si>
-    <t>Processeurs overclockés de 4e génération Intel® Core™ allant jusqu’au modèle i7</t>
-  </si>
-  <si>
     <t>Disque dur SATA de 1 To à 7 200 tr/min et 6 Gbit/s</t>
   </si>
   <si>
-    <t>Mémoire DDR4 de 8 Go 2133MHz (4Gox2)</t>
-  </si>
-  <si>
     <t>NVIDIA® GeForce® GTX 965M with 2GB GDDR5</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>IdSysExp</t>
   </si>
   <si>
-    <t>Processeur Intel® Celeron® G1840 (double cœur, 2 Mo de cache, 2,80 GHz, avec carte graphique Intel HD)</t>
-  </si>
-  <si>
     <t>DDR3L 4 Go3 à 1600 MHz</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>Carte graphique Intel® intégrée</t>
   </si>
   <si>
-    <t xml:space="preserve">Processeur Core i5 4e génération d'Intel </t>
-  </si>
-  <si>
     <t>8 Go de mémoire vive</t>
   </si>
   <si>
@@ -131,15 +119,9 @@
     <t>Nano SIM</t>
   </si>
   <si>
-    <t>Processeur octocœur 2.1GHz, 1.5GHz de 64 bits</t>
-  </si>
-  <si>
     <t>Micro-SIM (3FF)</t>
   </si>
   <si>
-    <t>Processeur 2,5 GHz Quadricoeur</t>
-  </si>
-  <si>
     <t>2 Go</t>
   </si>
   <si>
@@ -176,15 +158,9 @@
     <t>IPhone 6 Plus</t>
   </si>
   <si>
-    <t>WindowsSurface</t>
-  </si>
-  <si>
     <t>2Go</t>
   </si>
   <si>
-    <t>Processeur NVIDIA® TEGRA® 3 Quad Core CPU 1.30 GHz</t>
-  </si>
-  <si>
     <t>32 Go</t>
   </si>
   <si>
@@ -197,9 +173,6 @@
     <t>Galaxy Tab A</t>
   </si>
   <si>
-    <t>Processeur quadruple coeur APQ 8016 de 1,2 GHz</t>
-  </si>
-  <si>
     <t>1.5Go</t>
   </si>
   <si>
@@ -308,27 +281,12 @@
     <t>Mobile</t>
   </si>
   <si>
-    <t>Tablette</t>
-  </si>
-  <si>
     <t>XboxOne</t>
   </si>
   <si>
     <t>Xbox360</t>
   </si>
   <si>
-    <t>PCBureau</t>
-  </si>
-  <si>
-    <t>ConsoleSalon</t>
-  </si>
-  <si>
-    <t>ConsolePort</t>
-  </si>
-  <si>
-    <t>PCPortable</t>
-  </si>
-  <si>
     <t>Console Nintendo qui utilise le 3D</t>
   </si>
   <si>
@@ -338,9 +296,6 @@
     <t>Winchester</t>
   </si>
   <si>
-    <t>Processeur triple coeur 64-bit</t>
-  </si>
-  <si>
     <t>Console salon de Microsoft</t>
   </si>
   <si>
@@ -362,9 +317,6 @@
     <t>Ordinateur moins performante</t>
   </si>
   <si>
-    <t>Processeur multicœur de type IBM Power</t>
-  </si>
-  <si>
     <t>8-32 Go</t>
   </si>
   <si>
@@ -383,9 +335,6 @@
     <t>Wii U Mainboard PCB</t>
   </si>
   <si>
-    <t>Processeur Intel Core i5 de quatrième génération</t>
-  </si>
-  <si>
     <t>3 To</t>
   </si>
   <si>
@@ -395,9 +344,6 @@
     <t>Intel 20" EMC 2133</t>
   </si>
   <si>
-    <t xml:space="preserve">Processeur ARM11 MPCore-based dual-core </t>
-  </si>
-  <si>
     <t>128 Mo</t>
   </si>
   <si>
@@ -410,12 +356,6 @@
     <t>1 Go DDR3</t>
   </si>
   <si>
-    <t>Processeur Double coeur 1.3 GHz Cyclone (Arm v8-based)</t>
-  </si>
-  <si>
-    <t>Processeur Double coeur 1.4 GHz Cyclone (Arm v8-based)</t>
-  </si>
-  <si>
     <t>Exynos 7420</t>
   </si>
   <si>
@@ -456,6 +396,66 @@
   </si>
   <si>
     <t>Contient une plus grande memoire dû à sa carte mémoire</t>
+  </si>
+  <si>
+    <t>WinSurf</t>
+  </si>
+  <si>
+    <t>Intel® Celeron® G1840 (double cœur, 2 Mo de cache, 2,80 GHz, avec carte graphique Intel HD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core i5 4e génération d'Intel </t>
+  </si>
+  <si>
+    <t>2,5 GHz Quadricoeur</t>
+  </si>
+  <si>
+    <t>octocœur 2.1GHz de 64 bits</t>
+  </si>
+  <si>
+    <t>Double coeur 1.3 GHz Cyclone</t>
+  </si>
+  <si>
+    <t>Double coeur 1.4 GHz Cyclone</t>
+  </si>
+  <si>
+    <t>quadruple coeur APQ 8016 de 1,2 GHz</t>
+  </si>
+  <si>
+    <t>triple coeur 64-bit</t>
+  </si>
+  <si>
+    <t>multicœur de type IBM Power</t>
+  </si>
+  <si>
+    <t>Intel Core i5 de quatrième génération</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM11 MPCore-based dual-core </t>
+  </si>
+  <si>
+    <t>NVIDIA TEGRA 3 Quad Core CPU 1.30 GHz</t>
+  </si>
+  <si>
+    <t>4e génération Intel Core jusqu'à i7</t>
+  </si>
+  <si>
+    <t>DDR4 de 8 Go 2133MHz (4Gox2)</t>
+  </si>
+  <si>
+    <t>PCPort</t>
+  </si>
+  <si>
+    <t>PCBur</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>ConPort</t>
+  </si>
+  <si>
+    <t>ConSal</t>
   </si>
 </sst>
 </file>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +928,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -942,28 +942,28 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -971,34 +971,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1006,34 +1006,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>100</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1041,31 +1041,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1073,31 +1073,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1105,31 +1105,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
         <v>87</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1137,31 +1137,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1169,31 +1169,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1201,31 +1201,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K10" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1233,31 +1233,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1265,31 +1265,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="H12" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="K12" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1297,31 +1297,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1329,31 +1329,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K14" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1361,31 +1361,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K15" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1393,31 +1393,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
         <v>94</v>
       </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" t="s">
-        <v>109</v>
-      </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,31 +1425,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K17" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1457,28 +1457,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="K18" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1486,31 +1486,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="H19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K19" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1518,31 +1518,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="K20" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1570,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>